<commit_message>
Added project layout including Models with EF prepared navigation. Added StudentViewModel Added BusinessContext with StudentViewModel related functionality
</commit_message>
<xml_diff>
--- a/Tidsplan.xlsx
+++ b/Tidsplan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolai\Documents\GitHub\PlanAChaos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -276,9 +276,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kontor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -316,7 +316,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kontor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -388,7 +388,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kontor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -541,7 +541,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>